<commit_message>
Excel + Subarea -> Oficina 001
</commit_message>
<xml_diff>
--- a/imports/Consumo.xlsx
+++ b/imports/Consumo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Limpieza\LIMPIEZA_APP\sop_lavado_app\imports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F21DCE0-6B14-46FE-8C66-394CF845684E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F14E4ACB-D872-4B6A-AEC5-54D17AA6006A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,9 +68,6 @@
     <t>CM-DS-001</t>
   </si>
   <si>
-    <t>x 1m2 = 1 mL</t>
-  </si>
-  <si>
     <t>CM-DS-004</t>
   </si>
   <si>
@@ -161,9 +158,6 @@
     <t>uso</t>
   </si>
   <si>
-    <t>x 2m2 = 2 mL</t>
-  </si>
-  <si>
     <t>Consumo por área (m²)</t>
   </si>
   <si>
@@ -177,6 +171,12 @@
   </si>
   <si>
     <t>Consumo total solucion</t>
+  </si>
+  <si>
+    <t>x m2 = 1 mL</t>
+  </si>
+  <si>
+    <t>x m2 = 2 mL</t>
   </si>
 </sst>
 </file>
@@ -634,7 +634,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -655,12 +655,12 @@
       <c r="C1" s="9"/>
       <c r="D1" s="3"/>
       <c r="E1" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
       <c r="H1" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I1" s="13"/>
     </row>
@@ -678,19 +678,19 @@
         <v>4</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>25</v>
-      </c>
       <c r="G2" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="28.7" customHeight="1" x14ac:dyDescent="0.45">
@@ -704,7 +704,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="E3" s="2" t="str">
         <f>"CM"</f>
@@ -715,13 +715,13 @@
         <v>DS</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="28.7" customHeight="1" x14ac:dyDescent="0.45">
@@ -735,7 +735,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E4" s="2" t="str">
         <f t="shared" ref="E4:E10" si="0">"CM"</f>
@@ -746,13 +746,13 @@
         <v>DS</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="28.7" customHeight="1" x14ac:dyDescent="0.45">
@@ -777,18 +777,18 @@
         <v>DS</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="28.7" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
@@ -797,7 +797,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" s="2" t="str">
         <f t="shared" si="0"/>
@@ -808,18 +808,18 @@
         <v>DS</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="28.7" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2">
         <v>2</v>
@@ -828,7 +828,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" s="2" t="str">
         <f t="shared" si="0"/>
@@ -839,18 +839,18 @@
         <v>DS</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="28.7" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2">
         <v>6</v>
@@ -859,7 +859,7 @@
         <v>6</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="2" t="str">
         <f t="shared" si="0"/>
@@ -870,18 +870,18 @@
         <v>DS</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="28.7" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="2">
         <v>15</v>
@@ -890,7 +890,7 @@
         <v>6</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E9" s="2" t="str">
         <f t="shared" si="0"/>
@@ -901,24 +901,24 @@
         <v>DS</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="28.7" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="2">
         <v>500</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="2" t="str">
@@ -930,13 +930,13 @@
         <v>DS</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>